<commit_message>
Update DSP pin connection info.xlsx
</commit_message>
<xml_diff>
--- a/Design/Interface board/DSP pin connection info.xlsx
+++ b/Design/Interface board/DSP pin connection info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolai Fransen\Documents\GitHub\SemesterProjectPED2\Design\Interface board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4ACDE58C-5D5B-4AB9-A34C-36CEE4A9F60B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B372509B-A9DF-4924-8D95-1DD1B40B7EC3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7020" xr2:uid="{42574F33-9A8E-47BD-BFDC-F32E3330AB9B}"/>
   </bookViews>
@@ -464,8 +464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6A0220F-AB8A-4C9D-B8DD-91688DEC38F1}">
   <dimension ref="C4:K62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="F66" sqref="F66"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>